<commit_message>
recount | graphics fix
</commit_message>
<xml_diff>
--- a/economics.xlsx
+++ b/economics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dante\Desktop\matlab_service_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390FDDD5-338C-4EF6-9371-9D89FCA6A2AE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92E9945-3080-492D-8CA6-EFD7A573DB2B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1470" yWindow="2070" windowWidth="15375" windowHeight="7875" xr2:uid="{8EA334AC-AD76-46DB-9C49-41424F7A68FD}"/>
   </bookViews>
@@ -450,210 +450,210 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>0.99264316295971677</v>
+        <v>0.99192006418782341</v>
       </c>
       <c r="B2">
-        <v>312.12854923870168</v>
+        <v>309.04873793997916</v>
       </c>
       <c r="C2">
-        <v>362.06187047053118</v>
+        <v>358.78133278908865</v>
       </c>
       <c r="D2">
-        <v>28.023503117560537</v>
+        <v>27.841416924210222</v>
       </c>
       <c r="E2">
-        <v>32.507469817275108</v>
+        <v>32.321726780561526</v>
       </c>
       <c r="F2">
-        <v>3.9758227588960214E-2</v>
+        <v>3.9965666361292035E-2</v>
       </c>
       <c r="G2">
-        <v>0.81521457489878535</v>
+        <v>0.81809763313609429</v>
       </c>
       <c r="I2" s="1">
-        <v>157181907.30053833</v>
+        <v>156752862.81520677</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>0.4139209238145769</v>
+        <v>0.4157699305000736</v>
       </c>
       <c r="B3">
-        <v>0.64597277561684052</v>
+        <v>0.6361433039288471</v>
       </c>
       <c r="C3">
-        <v>50.458349840606303</v>
+        <v>50.649184543720224</v>
       </c>
       <c r="D3">
-        <v>5.8695471333003901E-2</v>
+        <v>5.8158574597714008E-2</v>
       </c>
       <c r="E3">
-        <v>4.5673255682130316</v>
+        <v>4.5899016244759911</v>
       </c>
       <c r="F3">
-        <v>4.9860037691294108E-2</v>
+        <v>4.9881197410415891E-2</v>
       </c>
       <c r="G3">
         <v>0.99999999999999978</v>
       </c>
       <c r="I3" s="1">
-        <v>271503998.20169044</v>
+        <v>271509454.42879027</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>0.99316192244026713</v>
+        <v>0.99302983780383469</v>
       </c>
       <c r="B4">
-        <v>493.86664959717427</v>
+        <v>493.29602857262228</v>
       </c>
       <c r="C4">
-        <v>543.91819938699996</v>
+        <v>543.36442854871268</v>
       </c>
       <c r="D4">
-        <v>44.355704928762293</v>
+        <v>44.176281137638618</v>
       </c>
       <c r="E4">
-        <v>48.851071378872909</v>
+        <v>48.660122922003112</v>
       </c>
       <c r="F4">
-        <v>3.965192037009159E-2</v>
+        <v>3.9668328896154847E-2</v>
       </c>
       <c r="G4">
-        <v>0.82352226720647748</v>
+        <v>0.82415680473372743</v>
       </c>
       <c r="I4" s="1">
-        <v>195565938.74943477</v>
+        <v>195140933.00936475</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.41652586069550268</v>
+        <v>0.41404917254056373</v>
       </c>
       <c r="B5">
-        <v>0.6639576655239523</v>
+        <v>0.6639152696053543</v>
       </c>
       <c r="C5">
-        <v>50.551224195967677</v>
+        <v>50.563002234733545</v>
       </c>
       <c r="D5">
-        <v>6.072643706412606E-2</v>
+        <v>6.0541303868019369E-2</v>
       </c>
       <c r="E5">
-        <v>4.5959897924439792</v>
+        <v>4.5757462277811571</v>
       </c>
       <c r="F5">
-        <v>5.0096548833874058E-2</v>
+        <v>4.9787033783367851E-2</v>
       </c>
       <c r="G5">
         <v>0.99999999999999967</v>
       </c>
       <c r="I5" s="1">
-        <v>271516432.55770355</v>
+        <v>271510276.55927974</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>0.995717538467773</v>
+        <v>0.99567415815144966</v>
       </c>
       <c r="B6">
-        <v>371.28333227393659</v>
+        <v>369.42540183886723</v>
       </c>
       <c r="C6">
-        <v>441.38330873923189</v>
+        <v>439.19591220053155</v>
       </c>
       <c r="D6">
-        <v>29.045113864712587</v>
+        <v>29.01900123566146</v>
       </c>
       <c r="E6">
-        <v>34.530570990423101</v>
+        <v>34.500907330906742</v>
       </c>
       <c r="F6">
-        <v>2.8388750620416812E-2</v>
+        <v>2.8590665341237886E-2</v>
       </c>
       <c r="G6">
-        <v>0.59019838056680141</v>
+        <v>0.59371893491124261</v>
       </c>
       <c r="I6" s="1">
-        <v>159878389.82417369</v>
+        <v>159815916.07801786</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.57847675237063201</v>
+        <v>0.58209682934979323</v>
       </c>
       <c r="B7">
-        <v>4.8775238906043796</v>
+        <v>4.9649386060883103</v>
       </c>
       <c r="C7">
-        <v>74.847242777130276</v>
+        <v>75.215080466535142</v>
       </c>
       <c r="D7">
-        <v>0.45771351048295372</v>
+        <v>0.46776842509143535</v>
       </c>
       <c r="E7">
-        <v>6.9929626255347639</v>
+        <v>7.0530153530681581</v>
       </c>
       <c r="F7">
-        <v>4.9605447423018111E-2</v>
+        <v>4.9717410754572852E-2</v>
       </c>
       <c r="G7">
         <v>0.99999999999999978</v>
       </c>
       <c r="I7" s="1">
-        <v>273031532.1993314</v>
+        <v>273069668.62597317</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>0.9956212750985336</v>
+        <v>0.99556162762487732</v>
       </c>
       <c r="B8">
-        <v>564.49647269560955</v>
+        <v>566.64059494631329</v>
       </c>
       <c r="C8">
-        <v>634.64599600256713</v>
+        <v>636.60514534259335</v>
       </c>
       <c r="D8">
-        <v>44.437786068882147</v>
+        <v>44.535249379858271</v>
       </c>
       <c r="E8">
-        <v>49.961139366962044</v>
+        <v>50.035471042989293</v>
       </c>
       <c r="F8">
-        <v>2.8407709183388363E-2</v>
+        <v>2.8487615738319504E-2</v>
       </c>
       <c r="G8">
-        <v>0.59844129554655845</v>
+        <v>0.6010650887573955</v>
       </c>
       <c r="I8" s="1">
-        <v>196062190.18067056</v>
+        <v>196284467.6907362</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>0.57766591287035729</v>
+        <v>0.57946601858870472</v>
       </c>
       <c r="B9">
-        <v>4.8409386677178077</v>
+        <v>4.8851188109151735</v>
       </c>
       <c r="C9">
-        <v>74.591452908538201</v>
+        <v>74.82581593753406</v>
       </c>
       <c r="D9">
-        <v>0.45602265835303157</v>
+        <v>0.46037536729605755</v>
       </c>
       <c r="E9">
-        <v>6.9929287664884594</v>
+        <v>7.0065957982973295</v>
       </c>
       <c r="F9">
-        <v>4.9696796493132661E-2</v>
+        <v>4.970788831558088E-2</v>
       </c>
       <c r="G9">
         <v>0.99999999999999956</v>
       </c>
       <c r="I9" s="1">
-        <v>273028006.62591213</v>
+        <v>273040941.80044872</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -661,28 +661,28 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0.79046967383042266</v>
+        <v>0.71716407280149264</v>
       </c>
       <c r="B11">
-        <v>36.702520893687101</v>
+        <v>23.220220952013833</v>
       </c>
       <c r="C11">
-        <v>97.354075055117278</v>
+        <v>84.359534252437641</v>
       </c>
       <c r="D11">
-        <v>3.7420017491995008</v>
+        <v>2.0494763040423134</v>
       </c>
       <c r="E11">
-        <v>9.9257247261892694</v>
+        <v>7.4457890313667434</v>
       </c>
       <c r="F11">
-        <v>5.2131866017909964E-2</v>
+        <v>4.6919995275545252E-2</v>
       </c>
       <c r="G11">
         <v>1</v>
       </c>
       <c r="I11" s="1">
-        <v>181835463.38630402</v>
+        <v>181606327.00365141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>